<commit_message>
Drawing and score implemented
</commit_message>
<xml_diff>
--- a/COMP3091 - Individual Project/Gantt chart.xlsx
+++ b/COMP3091 - Individual Project/Gantt chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farbas\Google Drive\COMP3091 - Individual Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farbas\Google Drive\Cleft-Lip-Individual-Project\COMP3091 - Individual Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -148,7 +148,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +173,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -461,7 +473,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -506,9 +518,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -528,6 +537,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -945,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1033,52 +1051,52 @@
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="44"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45" t="s">
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="38" t="s">
+      <c r="K3" s="48"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
       <c r="R3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="40" t="s">
+      <c r="S3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="40"/>
-      <c r="U3" s="40"/>
-      <c r="V3" s="40"/>
-      <c r="W3" s="38"/>
-      <c r="X3" s="41" t="s">
+      <c r="T3" s="42"/>
+      <c r="U3" s="42"/>
+      <c r="V3" s="42"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="Y3" s="42"/>
+      <c r="Y3" s="44"/>
     </row>
     <row r="4" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="36"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="4"/>
@@ -1104,10 +1122,10 @@
       <c r="Y4" s="22"/>
     </row>
     <row r="5" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="31"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="10"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -1133,10 +1151,10 @@
       <c r="Y5" s="23"/>
     </row>
     <row r="6" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="31"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -1162,7 +1180,7 @@
       <c r="Y6" s="23"/>
     </row>
     <row r="7" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="38" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="18"/>
@@ -1191,7 +1209,7 @@
       <c r="Y7" s="23"/>
     </row>
     <row r="8" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="38" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="18"/>
@@ -1200,7 +1218,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="8"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="32"/>
+      <c r="H8" s="31"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -1220,7 +1238,7 @@
       <c r="Y8" s="23"/>
     </row>
     <row r="9" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="38" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="18"/>
@@ -1229,7 +1247,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="33"/>
+      <c r="H9" s="32"/>
       <c r="I9" s="10"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -1249,7 +1267,7 @@
       <c r="Y9" s="23"/>
     </row>
     <row r="10" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="38" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="18"/>
@@ -1278,7 +1296,7 @@
       <c r="Y10" s="23"/>
     </row>
     <row r="11" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="38" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="18"/>
@@ -1307,7 +1325,7 @@
       <c r="Y11" s="23"/>
     </row>
     <row r="12" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="38" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="18"/>
@@ -1336,7 +1354,7 @@
       <c r="Y12" s="23"/>
     </row>
     <row r="13" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="39" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="18"/>
@@ -1362,7 +1380,7 @@
       <c r="Y13" s="23"/>
     </row>
     <row r="14" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="18"/>
@@ -1390,7 +1408,7 @@
       <c r="Y14" s="23"/>
     </row>
     <row r="15" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="39" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="18"/>
@@ -1411,7 +1429,7 @@
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="34"/>
+      <c r="T15" s="33"/>
       <c r="U15" s="10"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
@@ -1419,7 +1437,7 @@
       <c r="Y15" s="23"/>
     </row>
     <row r="16" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="38" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="18"/>
@@ -1448,7 +1466,7 @@
       <c r="Y16" s="23"/>
     </row>
     <row r="17" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="38" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="18"/>
@@ -1477,7 +1495,7 @@
       <c r="Y17" s="23"/>
     </row>
     <row r="18" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="18"/>
@@ -1498,15 +1516,15 @@
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="37"/>
+      <c r="T18" s="34"/>
+      <c r="U18" s="34"/>
+      <c r="V18" s="36"/>
       <c r="W18" s="8"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="23"/>
     </row>
     <row r="19" spans="1:25" ht="42.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="29" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="24"/>

</xml_diff>

<commit_message>
Code clean up/commenting, Windows/Android app packages for installation, project report, user/system manuals
</commit_message>
<xml_diff>
--- a/COMP3091 - Individual Project/Gantt chart.xlsx
+++ b/COMP3091 - Individual Project/Gantt chart.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -473,7 +473,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -518,12 +518,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
@@ -575,6 +569,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -963,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1051,52 +1048,52 @@
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="46"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="47" t="s">
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="48"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="40" t="s">
+      <c r="K3" s="46"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
       <c r="R3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="42" t="s">
+      <c r="S3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="42"/>
-      <c r="U3" s="42"/>
-      <c r="V3" s="42"/>
-      <c r="W3" s="40"/>
-      <c r="X3" s="43" t="s">
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="38"/>
+      <c r="X3" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="Y3" s="44"/>
+      <c r="Y3" s="42"/>
     </row>
     <row r="4" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="35"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="4"/>
@@ -1122,10 +1119,10 @@
       <c r="Y4" s="22"/>
     </row>
     <row r="5" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="30"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="10"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -1151,10 +1148,10 @@
       <c r="Y5" s="23"/>
     </row>
     <row r="6" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="30"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -1180,7 +1177,7 @@
       <c r="Y6" s="23"/>
     </row>
     <row r="7" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="36" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="18"/>
@@ -1209,7 +1206,7 @@
       <c r="Y7" s="23"/>
     </row>
     <row r="8" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="36" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="18"/>
@@ -1218,7 +1215,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="8"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="31"/>
+      <c r="H8" s="29"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -1238,7 +1235,7 @@
       <c r="Y8" s="23"/>
     </row>
     <row r="9" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="18"/>
@@ -1247,7 +1244,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="32"/>
+      <c r="H9" s="30"/>
       <c r="I9" s="10"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -1267,7 +1264,7 @@
       <c r="Y9" s="23"/>
     </row>
     <row r="10" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="36" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="18"/>
@@ -1296,7 +1293,7 @@
       <c r="Y10" s="23"/>
     </row>
     <row r="11" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="36" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="18"/>
@@ -1325,7 +1322,7 @@
       <c r="Y11" s="23"/>
     </row>
     <row r="12" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="36" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="18"/>
@@ -1354,7 +1351,7 @@
       <c r="Y12" s="23"/>
     </row>
     <row r="13" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="37" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="18"/>
@@ -1380,7 +1377,7 @@
       <c r="Y13" s="23"/>
     </row>
     <row r="14" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="36" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="18"/>
@@ -1408,7 +1405,7 @@
       <c r="Y14" s="23"/>
     </row>
     <row r="15" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="37" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="18"/>
@@ -1429,7 +1426,7 @@
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="33"/>
+      <c r="T15" s="31"/>
       <c r="U15" s="10"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
@@ -1437,7 +1434,7 @@
       <c r="Y15" s="23"/>
     </row>
     <row r="16" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="36" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="18"/>
@@ -1466,7 +1463,7 @@
       <c r="Y16" s="23"/>
     </row>
     <row r="17" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="36" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="18"/>
@@ -1495,7 +1492,7 @@
       <c r="Y17" s="23"/>
     </row>
     <row r="18" spans="1:25" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="36" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="18"/>
@@ -1516,15 +1513,15 @@
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
-      <c r="T18" s="34"/>
-      <c r="U18" s="34"/>
-      <c r="V18" s="36"/>
+      <c r="T18" s="32"/>
+      <c r="U18" s="32"/>
+      <c r="V18" s="34"/>
       <c r="W18" s="8"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="23"/>
     </row>
     <row r="19" spans="1:25" ht="42.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="48" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="24"/>

</xml_diff>